<commit_message>
put all combinedData in one xlsx file. checking still needed
</commit_message>
<xml_diff>
--- a/data/fiber/1985 fibers.xlsx
+++ b/data/fiber/1985 fibers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahhchu/Desktop/R/USCottonWeather/data/fiber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838F3F9D-6C98-E043-A806-9A332D2F0A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478E506E-D9B5-0D4F-BCA3-6C68C3B3B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6660" yWindow="1600" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,7 +198,7 @@
     <t>Thrall, TX</t>
   </si>
   <si>
-    <t>str_mot</t>
+    <t>str_mpt</t>
   </si>
 </sst>
 </file>

</xml_diff>